<commit_message>
Update weekly schedule and info
</commit_message>
<xml_diff>
--- a/Input Data/Update Elo/CFB_Sch_23-24 (Completed).xlsx
+++ b/Input Data/Update Elo/CFB_Sch_23-24 (Completed).xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H725"/>
+  <dimension ref="A1:H793"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20747,6 +20747,1910 @@
         <v>0</v>
       </c>
     </row>
+    <row r="726">
+      <c r="A726" t="n">
+        <v>13</v>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Eastern Michigan</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>Akron</t>
+        </is>
+      </c>
+      <c r="D726" t="inlineStr"/>
+      <c r="E726" t="n">
+        <v>0</v>
+      </c>
+      <c r="F726" t="n">
+        <v>3</v>
+      </c>
+      <c r="G726" t="n">
+        <v>1</v>
+      </c>
+      <c r="H726" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="n">
+        <v>13</v>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Northern Illinois</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>Western Michigan</t>
+        </is>
+      </c>
+      <c r="D727" t="inlineStr"/>
+      <c r="E727" t="n">
+        <v>0</v>
+      </c>
+      <c r="F727" t="n">
+        <v>24</v>
+      </c>
+      <c r="G727" t="n">
+        <v>1</v>
+      </c>
+      <c r="H727" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="n">
+        <v>13</v>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Bowling Green</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>Toledo</t>
+        </is>
+      </c>
+      <c r="D728" t="inlineStr"/>
+      <c r="E728" t="n">
+        <v>0</v>
+      </c>
+      <c r="F728" t="n">
+        <v>1</v>
+      </c>
+      <c r="G728" t="n">
+        <v>0</v>
+      </c>
+      <c r="H728" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="n">
+        <v>13</v>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Miami (OH)</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>Buffalo</t>
+        </is>
+      </c>
+      <c r="D729" t="inlineStr"/>
+      <c r="E729" t="n">
+        <v>0</v>
+      </c>
+      <c r="F729" t="n">
+        <v>13</v>
+      </c>
+      <c r="G729" t="n">
+        <v>1</v>
+      </c>
+      <c r="H729" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="n">
+        <v>13</v>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Ohio</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>Central Michigan</t>
+        </is>
+      </c>
+      <c r="D730" t="inlineStr"/>
+      <c r="E730" t="n">
+        <v>0</v>
+      </c>
+      <c r="F730" t="n">
+        <v>14</v>
+      </c>
+      <c r="G730" t="n">
+        <v>1</v>
+      </c>
+      <c r="H730" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="n">
+        <v>13</v>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Pittsburgh</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>Boston College</t>
+        </is>
+      </c>
+      <c r="D731" t="inlineStr"/>
+      <c r="E731" t="n">
+        <v>0</v>
+      </c>
+      <c r="F731" t="n">
+        <v>8</v>
+      </c>
+      <c r="G731" t="n">
+        <v>1</v>
+      </c>
+      <c r="H731" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="n">
+        <v>13</v>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Texas-San Antonio</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>South Florida</t>
+        </is>
+      </c>
+      <c r="D732" t="inlineStr"/>
+      <c r="E732" t="n">
+        <v>0</v>
+      </c>
+      <c r="F732" t="n">
+        <v>28</v>
+      </c>
+      <c r="G732" t="n">
+        <v>1</v>
+      </c>
+      <c r="H732" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="n">
+        <v>13</v>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Washington State</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>Colorado</t>
+        </is>
+      </c>
+      <c r="D733" t="inlineStr"/>
+      <c r="E733" t="n">
+        <v>0</v>
+      </c>
+      <c r="F733" t="n">
+        <v>42</v>
+      </c>
+      <c r="G733" t="n">
+        <v>1</v>
+      </c>
+      <c r="H733" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="n">
+        <v>13</v>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Alabama</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>Chattanooga</t>
+        </is>
+      </c>
+      <c r="D734" t="inlineStr"/>
+      <c r="E734" t="n">
+        <v>0</v>
+      </c>
+      <c r="F734" t="n">
+        <v>56</v>
+      </c>
+      <c r="G734" t="n">
+        <v>1</v>
+      </c>
+      <c r="H734" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="n">
+        <v>13</v>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Alabama-Birmingham</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>Temple</t>
+        </is>
+      </c>
+      <c r="D735" t="inlineStr"/>
+      <c r="E735" t="n">
+        <v>0</v>
+      </c>
+      <c r="F735" t="n">
+        <v>10</v>
+      </c>
+      <c r="G735" t="n">
+        <v>1</v>
+      </c>
+      <c r="H735" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="n">
+        <v>13</v>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>James Madison</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>Appalachian State</t>
+        </is>
+      </c>
+      <c r="D736" t="inlineStr"/>
+      <c r="E736" t="n">
+        <v>0</v>
+      </c>
+      <c r="F736" t="n">
+        <v>3</v>
+      </c>
+      <c r="G736" t="n">
+        <v>0</v>
+      </c>
+      <c r="H736" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="n">
+        <v>13</v>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Arizona</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>Utah</t>
+        </is>
+      </c>
+      <c r="D737" t="inlineStr"/>
+      <c r="E737" t="n">
+        <v>0</v>
+      </c>
+      <c r="F737" t="n">
+        <v>24</v>
+      </c>
+      <c r="G737" t="n">
+        <v>1</v>
+      </c>
+      <c r="H737" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="n">
+        <v>13</v>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Arkansas</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>Florida International</t>
+        </is>
+      </c>
+      <c r="D738" t="inlineStr"/>
+      <c r="E738" t="n">
+        <v>0</v>
+      </c>
+      <c r="F738" t="n">
+        <v>24</v>
+      </c>
+      <c r="G738" t="n">
+        <v>1</v>
+      </c>
+      <c r="H738" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="n">
+        <v>13</v>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Arkansas State</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>Texas State</t>
+        </is>
+      </c>
+      <c r="D739" t="inlineStr"/>
+      <c r="E739" t="n">
+        <v>0</v>
+      </c>
+      <c r="F739" t="n">
+        <v>46</v>
+      </c>
+      <c r="G739" t="n">
+        <v>1</v>
+      </c>
+      <c r="H739" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="n">
+        <v>13</v>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Army</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>Coastal Carolina</t>
+        </is>
+      </c>
+      <c r="D740" t="inlineStr"/>
+      <c r="E740" t="n">
+        <v>0</v>
+      </c>
+      <c r="F740" t="n">
+        <v>7</v>
+      </c>
+      <c r="G740" t="n">
+        <v>1</v>
+      </c>
+      <c r="H740" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="n">
+        <v>13</v>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Ball State</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>Kent State</t>
+        </is>
+      </c>
+      <c r="D741" t="inlineStr"/>
+      <c r="E741" t="n">
+        <v>0</v>
+      </c>
+      <c r="F741" t="n">
+        <v>31</v>
+      </c>
+      <c r="G741" t="n">
+        <v>1</v>
+      </c>
+      <c r="H741" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="n">
+        <v>13</v>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Utah State</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>Boise State</t>
+        </is>
+      </c>
+      <c r="D742" t="inlineStr"/>
+      <c r="E742" t="n">
+        <v>0</v>
+      </c>
+      <c r="F742" t="n">
+        <v>35</v>
+      </c>
+      <c r="G742" t="n">
+        <v>0</v>
+      </c>
+      <c r="H742" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="n">
+        <v>13</v>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Stanford</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>California</t>
+        </is>
+      </c>
+      <c r="D743" t="inlineStr"/>
+      <c r="E743" t="n">
+        <v>0</v>
+      </c>
+      <c r="F743" t="n">
+        <v>12</v>
+      </c>
+      <c r="G743" t="n">
+        <v>0</v>
+      </c>
+      <c r="H743" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="n">
+        <v>13</v>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Clemson</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>North Carolina</t>
+        </is>
+      </c>
+      <c r="D744" t="inlineStr"/>
+      <c r="E744" t="n">
+        <v>0</v>
+      </c>
+      <c r="F744" t="n">
+        <v>11</v>
+      </c>
+      <c r="G744" t="n">
+        <v>1</v>
+      </c>
+      <c r="H744" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="n">
+        <v>13</v>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Colorado State</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>Nevada</t>
+        </is>
+      </c>
+      <c r="D745" t="inlineStr"/>
+      <c r="E745" t="n">
+        <v>0</v>
+      </c>
+      <c r="F745" t="n">
+        <v>10</v>
+      </c>
+      <c r="G745" t="n">
+        <v>1</v>
+      </c>
+      <c r="H745" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="n">
+        <v>13</v>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Connecticut</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>Sacred Heart</t>
+        </is>
+      </c>
+      <c r="D746" t="inlineStr"/>
+      <c r="E746" t="n">
+        <v>0</v>
+      </c>
+      <c r="F746" t="n">
+        <v>28</v>
+      </c>
+      <c r="G746" t="n">
+        <v>1</v>
+      </c>
+      <c r="H746" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="n">
+        <v>13</v>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Florida State</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>North Alabama</t>
+        </is>
+      </c>
+      <c r="D747" t="inlineStr"/>
+      <c r="E747" t="n">
+        <v>0</v>
+      </c>
+      <c r="F747" t="n">
+        <v>45</v>
+      </c>
+      <c r="G747" t="n">
+        <v>1</v>
+      </c>
+      <c r="H747" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="n">
+        <v>13</v>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Tennessee</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>Georgia</t>
+        </is>
+      </c>
+      <c r="D748" t="inlineStr"/>
+      <c r="E748" t="n">
+        <v>0</v>
+      </c>
+      <c r="F748" t="n">
+        <v>28</v>
+      </c>
+      <c r="G748" t="n">
+        <v>0</v>
+      </c>
+      <c r="H748" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="n">
+        <v>13</v>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Georgia Tech</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>Syracuse</t>
+        </is>
+      </c>
+      <c r="D749" t="inlineStr"/>
+      <c r="E749" t="n">
+        <v>0</v>
+      </c>
+      <c r="F749" t="n">
+        <v>9</v>
+      </c>
+      <c r="G749" t="n">
+        <v>1</v>
+      </c>
+      <c r="H749" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="n">
+        <v>13</v>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Iowa</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>Illinois</t>
+        </is>
+      </c>
+      <c r="D750" t="inlineStr"/>
+      <c r="E750" t="n">
+        <v>0</v>
+      </c>
+      <c r="F750" t="n">
+        <v>2</v>
+      </c>
+      <c r="G750" t="n">
+        <v>1</v>
+      </c>
+      <c r="H750" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="n">
+        <v>13</v>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Jacksonville State</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>Louisiana Tech</t>
+        </is>
+      </c>
+      <c r="D751" t="inlineStr"/>
+      <c r="E751" t="n">
+        <v>0</v>
+      </c>
+      <c r="F751" t="n">
+        <v>39</v>
+      </c>
+      <c r="G751" t="n">
+        <v>1</v>
+      </c>
+      <c r="H751" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="n">
+        <v>13</v>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Kansas</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>Kansas State</t>
+        </is>
+      </c>
+      <c r="D752" t="inlineStr"/>
+      <c r="E752" t="n">
+        <v>0</v>
+      </c>
+      <c r="F752" t="n">
+        <v>4</v>
+      </c>
+      <c r="G752" t="n">
+        <v>0</v>
+      </c>
+      <c r="H752" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="n">
+        <v>13</v>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Liberty</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>Massachusetts</t>
+        </is>
+      </c>
+      <c r="D753" t="inlineStr"/>
+      <c r="E753" t="n">
+        <v>0</v>
+      </c>
+      <c r="F753" t="n">
+        <v>24</v>
+      </c>
+      <c r="G753" t="n">
+        <v>1</v>
+      </c>
+      <c r="H753" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="n">
+        <v>13</v>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Louisiana State</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>Georgia State</t>
+        </is>
+      </c>
+      <c r="D754" t="inlineStr"/>
+      <c r="E754" t="n">
+        <v>0</v>
+      </c>
+      <c r="F754" t="n">
+        <v>42</v>
+      </c>
+      <c r="G754" t="n">
+        <v>1</v>
+      </c>
+      <c r="H754" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="n">
+        <v>13</v>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Miami (FL)</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>Louisville</t>
+        </is>
+      </c>
+      <c r="D755" t="inlineStr"/>
+      <c r="E755" t="n">
+        <v>0</v>
+      </c>
+      <c r="F755" t="n">
+        <v>7</v>
+      </c>
+      <c r="G755" t="n">
+        <v>0</v>
+      </c>
+      <c r="H755" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="n">
+        <v>13</v>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Maryland</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>Michigan</t>
+        </is>
+      </c>
+      <c r="D756" t="inlineStr"/>
+      <c r="E756" t="n">
+        <v>0</v>
+      </c>
+      <c r="F756" t="n">
+        <v>7</v>
+      </c>
+      <c r="G756" t="n">
+        <v>0</v>
+      </c>
+      <c r="H756" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="n">
+        <v>13</v>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Indiana</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>Michigan State</t>
+        </is>
+      </c>
+      <c r="D757" t="inlineStr"/>
+      <c r="E757" t="n">
+        <v>0</v>
+      </c>
+      <c r="F757" t="n">
+        <v>3</v>
+      </c>
+      <c r="G757" t="n">
+        <v>0</v>
+      </c>
+      <c r="H757" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="n">
+        <v>13</v>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Middle Tennessee State</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>Texas-El Paso</t>
+        </is>
+      </c>
+      <c r="D758" t="inlineStr"/>
+      <c r="E758" t="n">
+        <v>0</v>
+      </c>
+      <c r="F758" t="n">
+        <v>4</v>
+      </c>
+      <c r="G758" t="n">
+        <v>1</v>
+      </c>
+      <c r="H758" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="n">
+        <v>13</v>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Mississippi</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>Louisiana-Monroe</t>
+        </is>
+      </c>
+      <c r="D759" t="inlineStr"/>
+      <c r="E759" t="n">
+        <v>0</v>
+      </c>
+      <c r="F759" t="n">
+        <v>32</v>
+      </c>
+      <c r="G759" t="n">
+        <v>1</v>
+      </c>
+      <c r="H759" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="n">
+        <v>13</v>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Mississippi State</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>Southern Mississippi</t>
+        </is>
+      </c>
+      <c r="D760" t="inlineStr"/>
+      <c r="E760" t="n">
+        <v>0</v>
+      </c>
+      <c r="F760" t="n">
+        <v>21</v>
+      </c>
+      <c r="G760" t="n">
+        <v>1</v>
+      </c>
+      <c r="H760" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="n">
+        <v>13</v>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Missouri</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>Florida</t>
+        </is>
+      </c>
+      <c r="D761" t="inlineStr"/>
+      <c r="E761" t="n">
+        <v>0</v>
+      </c>
+      <c r="F761" t="n">
+        <v>2</v>
+      </c>
+      <c r="G761" t="n">
+        <v>1</v>
+      </c>
+      <c r="H761" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="n">
+        <v>13</v>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Navy</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>East Carolina</t>
+        </is>
+      </c>
+      <c r="D762" t="inlineStr"/>
+      <c r="E762" t="n">
+        <v>0</v>
+      </c>
+      <c r="F762" t="n">
+        <v>10</v>
+      </c>
+      <c r="G762" t="n">
+        <v>1</v>
+      </c>
+      <c r="H762" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="n">
+        <v>13</v>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Air Force</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>Nevada-Las Vegas</t>
+        </is>
+      </c>
+      <c r="D763" t="inlineStr"/>
+      <c r="E763" t="n">
+        <v>0</v>
+      </c>
+      <c r="F763" t="n">
+        <v>4</v>
+      </c>
+      <c r="G763" t="n">
+        <v>0</v>
+      </c>
+      <c r="H763" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="n">
+        <v>13</v>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Fresno State</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>New Mexico</t>
+        </is>
+      </c>
+      <c r="D764" t="inlineStr"/>
+      <c r="E764" t="n">
+        <v>0</v>
+      </c>
+      <c r="F764" t="n">
+        <v>8</v>
+      </c>
+      <c r="G764" t="n">
+        <v>0</v>
+      </c>
+      <c r="H764" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="n">
+        <v>13</v>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Auburn</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>New Mexico State</t>
+        </is>
+      </c>
+      <c r="D765" t="inlineStr"/>
+      <c r="E765" t="n">
+        <v>0</v>
+      </c>
+      <c r="F765" t="n">
+        <v>21</v>
+      </c>
+      <c r="G765" t="n">
+        <v>0</v>
+      </c>
+      <c r="H765" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="n">
+        <v>13</v>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Virginia Tech</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>North Carolina State</t>
+        </is>
+      </c>
+      <c r="D766" t="inlineStr"/>
+      <c r="E766" t="n">
+        <v>0</v>
+      </c>
+      <c r="F766" t="n">
+        <v>7</v>
+      </c>
+      <c r="G766" t="n">
+        <v>0</v>
+      </c>
+      <c r="H766" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="n">
+        <v>13</v>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Tulsa</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>North Texas</t>
+        </is>
+      </c>
+      <c r="D767" t="inlineStr"/>
+      <c r="E767" t="n">
+        <v>0</v>
+      </c>
+      <c r="F767" t="n">
+        <v>7</v>
+      </c>
+      <c r="G767" t="n">
+        <v>0</v>
+      </c>
+      <c r="H767" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="n">
+        <v>13</v>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Northwestern</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>Purdue</t>
+        </is>
+      </c>
+      <c r="D768" t="inlineStr"/>
+      <c r="E768" t="n">
+        <v>0</v>
+      </c>
+      <c r="F768" t="n">
+        <v>8</v>
+      </c>
+      <c r="G768" t="n">
+        <v>1</v>
+      </c>
+      <c r="H768" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="n">
+        <v>13</v>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Notre Dame</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>Wake Forest</t>
+        </is>
+      </c>
+      <c r="D769" t="inlineStr"/>
+      <c r="E769" t="n">
+        <v>0</v>
+      </c>
+      <c r="F769" t="n">
+        <v>38</v>
+      </c>
+      <c r="G769" t="n">
+        <v>1</v>
+      </c>
+      <c r="H769" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="n">
+        <v>13</v>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Ohio State</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>Minnesota</t>
+        </is>
+      </c>
+      <c r="D770" t="inlineStr"/>
+      <c r="E770" t="n">
+        <v>0</v>
+      </c>
+      <c r="F770" t="n">
+        <v>34</v>
+      </c>
+      <c r="G770" t="n">
+        <v>1</v>
+      </c>
+      <c r="H770" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="n">
+        <v>13</v>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Brigham Young</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>Oklahoma</t>
+        </is>
+      </c>
+      <c r="D771" t="inlineStr"/>
+      <c r="E771" t="n">
+        <v>0</v>
+      </c>
+      <c r="F771" t="n">
+        <v>7</v>
+      </c>
+      <c r="G771" t="n">
+        <v>0</v>
+      </c>
+      <c r="H771" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="n">
+        <v>13</v>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Houston</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>Oklahoma State</t>
+        </is>
+      </c>
+      <c r="D772" t="inlineStr"/>
+      <c r="E772" t="n">
+        <v>0</v>
+      </c>
+      <c r="F772" t="n">
+        <v>13</v>
+      </c>
+      <c r="G772" t="n">
+        <v>0</v>
+      </c>
+      <c r="H772" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="n">
+        <v>13</v>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Georgia Southern</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>Old Dominion</t>
+        </is>
+      </c>
+      <c r="D773" t="inlineStr"/>
+      <c r="E773" t="n">
+        <v>0</v>
+      </c>
+      <c r="F773" t="n">
+        <v>3</v>
+      </c>
+      <c r="G773" t="n">
+        <v>0</v>
+      </c>
+      <c r="H773" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="n">
+        <v>13</v>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Arizona State</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>Oregon</t>
+        </is>
+      </c>
+      <c r="D774" t="inlineStr"/>
+      <c r="E774" t="n">
+        <v>0</v>
+      </c>
+      <c r="F774" t="n">
+        <v>36</v>
+      </c>
+      <c r="G774" t="n">
+        <v>0</v>
+      </c>
+      <c r="H774" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="n">
+        <v>13</v>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Penn State</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>Rutgers</t>
+        </is>
+      </c>
+      <c r="D775" t="inlineStr"/>
+      <c r="E775" t="n">
+        <v>0</v>
+      </c>
+      <c r="F775" t="n">
+        <v>21</v>
+      </c>
+      <c r="G775" t="n">
+        <v>1</v>
+      </c>
+      <c r="H775" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="n">
+        <v>13</v>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Charlotte</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>Rice</t>
+        </is>
+      </c>
+      <c r="D776" t="inlineStr"/>
+      <c r="E776" t="n">
+        <v>0</v>
+      </c>
+      <c r="F776" t="n">
+        <v>21</v>
+      </c>
+      <c r="G776" t="n">
+        <v>0</v>
+      </c>
+      <c r="H776" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="n">
+        <v>13</v>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>San Jose State</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>San Diego State</t>
+        </is>
+      </c>
+      <c r="D777" t="inlineStr"/>
+      <c r="E777" t="n">
+        <v>0</v>
+      </c>
+      <c r="F777" t="n">
+        <v>11</v>
+      </c>
+      <c r="G777" t="n">
+        <v>1</v>
+      </c>
+      <c r="H777" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="n">
+        <v>13</v>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>South Alabama</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>Marshall</t>
+        </is>
+      </c>
+      <c r="D778" t="inlineStr"/>
+      <c r="E778" t="n">
+        <v>0</v>
+      </c>
+      <c r="F778" t="n">
+        <v>28</v>
+      </c>
+      <c r="G778" t="n">
+        <v>1</v>
+      </c>
+      <c r="H778" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="n">
+        <v>13</v>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>South Carolina</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>Kentucky</t>
+        </is>
+      </c>
+      <c r="D779" t="inlineStr"/>
+      <c r="E779" t="n">
+        <v>0</v>
+      </c>
+      <c r="F779" t="n">
+        <v>3</v>
+      </c>
+      <c r="G779" t="n">
+        <v>1</v>
+      </c>
+      <c r="H779" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="n">
+        <v>13</v>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Memphis</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>Southern Methodist</t>
+        </is>
+      </c>
+      <c r="D780" t="inlineStr"/>
+      <c r="E780" t="n">
+        <v>0</v>
+      </c>
+      <c r="F780" t="n">
+        <v>4</v>
+      </c>
+      <c r="G780" t="n">
+        <v>0</v>
+      </c>
+      <c r="H780" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="n">
+        <v>13</v>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Iowa State</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>Texas</t>
+        </is>
+      </c>
+      <c r="D781" t="inlineStr"/>
+      <c r="E781" t="n">
+        <v>0</v>
+      </c>
+      <c r="F781" t="n">
+        <v>10</v>
+      </c>
+      <c r="G781" t="n">
+        <v>0</v>
+      </c>
+      <c r="H781" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="n">
+        <v>13</v>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Texas A&amp;M</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>Abilene Christian</t>
+        </is>
+      </c>
+      <c r="D782" t="inlineStr"/>
+      <c r="E782" t="n">
+        <v>0</v>
+      </c>
+      <c r="F782" t="n">
+        <v>28</v>
+      </c>
+      <c r="G782" t="n">
+        <v>1</v>
+      </c>
+      <c r="H782" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="n">
+        <v>13</v>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Texas Christian</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>Baylor</t>
+        </is>
+      </c>
+      <c r="D783" t="inlineStr"/>
+      <c r="E783" t="n">
+        <v>0</v>
+      </c>
+      <c r="F783" t="n">
+        <v>25</v>
+      </c>
+      <c r="G783" t="n">
+        <v>1</v>
+      </c>
+      <c r="H783" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="n">
+        <v>13</v>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Texas Tech</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>Central Florida</t>
+        </is>
+      </c>
+      <c r="D784" t="inlineStr"/>
+      <c r="E784" t="n">
+        <v>0</v>
+      </c>
+      <c r="F784" t="n">
+        <v>1</v>
+      </c>
+      <c r="G784" t="n">
+        <v>1</v>
+      </c>
+      <c r="H784" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="n">
+        <v>13</v>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Troy</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>Louisiana</t>
+        </is>
+      </c>
+      <c r="D785" t="inlineStr"/>
+      <c r="E785" t="n">
+        <v>0</v>
+      </c>
+      <c r="F785" t="n">
+        <v>7</v>
+      </c>
+      <c r="G785" t="n">
+        <v>1</v>
+      </c>
+      <c r="H785" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="n">
+        <v>13</v>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Florida Atlantic</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>Tulane</t>
+        </is>
+      </c>
+      <c r="D786" t="inlineStr"/>
+      <c r="E786" t="n">
+        <v>0</v>
+      </c>
+      <c r="F786" t="n">
+        <v>16</v>
+      </c>
+      <c r="G786" t="n">
+        <v>0</v>
+      </c>
+      <c r="H786" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="n">
+        <v>13</v>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Southern California</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>UCLA</t>
+        </is>
+      </c>
+      <c r="D787" t="inlineStr"/>
+      <c r="E787" t="n">
+        <v>0</v>
+      </c>
+      <c r="F787" t="n">
+        <v>18</v>
+      </c>
+      <c r="G787" t="n">
+        <v>0</v>
+      </c>
+      <c r="H787" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="n">
+        <v>13</v>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Virginia</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>Duke</t>
+        </is>
+      </c>
+      <c r="D788" t="inlineStr"/>
+      <c r="E788" t="n">
+        <v>0</v>
+      </c>
+      <c r="F788" t="n">
+        <v>3</v>
+      </c>
+      <c r="G788" t="n">
+        <v>1</v>
+      </c>
+      <c r="H788" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="n">
+        <v>13</v>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Oregon State</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>Washington</t>
+        </is>
+      </c>
+      <c r="D789" t="inlineStr"/>
+      <c r="E789" t="n">
+        <v>0</v>
+      </c>
+      <c r="F789" t="n">
+        <v>2</v>
+      </c>
+      <c r="G789" t="n">
+        <v>0</v>
+      </c>
+      <c r="H789" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="n">
+        <v>13</v>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>West Virginia</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>Cincinnati</t>
+        </is>
+      </c>
+      <c r="D790" t="inlineStr"/>
+      <c r="E790" t="n">
+        <v>0</v>
+      </c>
+      <c r="F790" t="n">
+        <v>21</v>
+      </c>
+      <c r="G790" t="n">
+        <v>1</v>
+      </c>
+      <c r="H790" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="n">
+        <v>13</v>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Western Kentucky</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>Sam Houston</t>
+        </is>
+      </c>
+      <c r="D791" t="inlineStr"/>
+      <c r="E791" t="n">
+        <v>0</v>
+      </c>
+      <c r="F791" t="n">
+        <v>5</v>
+      </c>
+      <c r="G791" t="n">
+        <v>1</v>
+      </c>
+      <c r="H791" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="n">
+        <v>13</v>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Wisconsin</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>Nebraska</t>
+        </is>
+      </c>
+      <c r="D792" t="inlineStr"/>
+      <c r="E792" t="n">
+        <v>0</v>
+      </c>
+      <c r="F792" t="n">
+        <v>7</v>
+      </c>
+      <c r="G792" t="n">
+        <v>1</v>
+      </c>
+      <c r="H792" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="n">
+        <v>13</v>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Wyoming</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>Hawaii</t>
+        </is>
+      </c>
+      <c r="D793" t="inlineStr"/>
+      <c r="E793" t="n">
+        <v>0</v>
+      </c>
+      <c r="F793" t="n">
+        <v>33</v>
+      </c>
+      <c r="G793" t="n">
+        <v>1</v>
+      </c>
+      <c r="H793" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update functionality for custom scenarios and update elo for end of regular season results
</commit_message>
<xml_diff>
--- a/Input Data/Update Elo/CFB_Sch_23-24 (Completed).xlsx
+++ b/Input Data/Update Elo/CFB_Sch_23-24 (Completed).xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H793"/>
+  <dimension ref="A1:H858"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22651,6 +22651,1826 @@
         <v>0</v>
       </c>
     </row>
+    <row r="794">
+      <c r="A794" t="n">
+        <v>14</v>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Western Michigan</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>Bowling Green</t>
+        </is>
+      </c>
+      <c r="D794" t="inlineStr"/>
+      <c r="E794" t="n">
+        <v>0</v>
+      </c>
+      <c r="F794" t="n">
+        <v>24</v>
+      </c>
+      <c r="G794" t="n">
+        <v>0</v>
+      </c>
+      <c r="H794" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="n">
+        <v>14</v>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Buffalo</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>Eastern Michigan</t>
+        </is>
+      </c>
+      <c r="D795" t="inlineStr"/>
+      <c r="E795" t="n">
+        <v>0</v>
+      </c>
+      <c r="F795" t="n">
+        <v>13</v>
+      </c>
+      <c r="G795" t="n">
+        <v>0</v>
+      </c>
+      <c r="H795" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="n">
+        <v>14</v>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Mississippi State</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>Mississippi</t>
+        </is>
+      </c>
+      <c r="D796" t="inlineStr"/>
+      <c r="E796" t="n">
+        <v>0</v>
+      </c>
+      <c r="F796" t="n">
+        <v>10</v>
+      </c>
+      <c r="G796" t="n">
+        <v>0</v>
+      </c>
+      <c r="H796" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="n">
+        <v>14</v>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Boise State</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>Air Force</t>
+        </is>
+      </c>
+      <c r="D797" t="inlineStr"/>
+      <c r="E797" t="n">
+        <v>0</v>
+      </c>
+      <c r="F797" t="n">
+        <v>8</v>
+      </c>
+      <c r="G797" t="n">
+        <v>1</v>
+      </c>
+      <c r="H797" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="n">
+        <v>14</v>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Nebraska</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>Iowa</t>
+        </is>
+      </c>
+      <c r="D798" t="inlineStr"/>
+      <c r="E798" t="n">
+        <v>0</v>
+      </c>
+      <c r="F798" t="n">
+        <v>3</v>
+      </c>
+      <c r="G798" t="n">
+        <v>0</v>
+      </c>
+      <c r="H798" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="n">
+        <v>14</v>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Temple</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>Memphis</t>
+        </is>
+      </c>
+      <c r="D799" t="inlineStr"/>
+      <c r="E799" t="n">
+        <v>0</v>
+      </c>
+      <c r="F799" t="n">
+        <v>24</v>
+      </c>
+      <c r="G799" t="n">
+        <v>0</v>
+      </c>
+      <c r="H799" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="n">
+        <v>14</v>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Boston College</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>Miami (FL)</t>
+        </is>
+      </c>
+      <c r="D800" t="inlineStr"/>
+      <c r="E800" t="n">
+        <v>0</v>
+      </c>
+      <c r="F800" t="n">
+        <v>25</v>
+      </c>
+      <c r="G800" t="n">
+        <v>0</v>
+      </c>
+      <c r="H800" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="n">
+        <v>14</v>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Arkansas</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>Missouri</t>
+        </is>
+      </c>
+      <c r="D801" t="inlineStr"/>
+      <c r="E801" t="n">
+        <v>0</v>
+      </c>
+      <c r="F801" t="n">
+        <v>34</v>
+      </c>
+      <c r="G801" t="n">
+        <v>0</v>
+      </c>
+      <c r="H801" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="n">
+        <v>14</v>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Akron</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>Ohio</t>
+        </is>
+      </c>
+      <c r="D802" t="inlineStr"/>
+      <c r="E802" t="n">
+        <v>0</v>
+      </c>
+      <c r="F802" t="n">
+        <v>11</v>
+      </c>
+      <c r="G802" t="n">
+        <v>0</v>
+      </c>
+      <c r="H802" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="n">
+        <v>14</v>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Oklahoma</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>Texas Christian</t>
+        </is>
+      </c>
+      <c r="D803" t="inlineStr"/>
+      <c r="E803" t="n">
+        <v>0</v>
+      </c>
+      <c r="F803" t="n">
+        <v>24</v>
+      </c>
+      <c r="G803" t="n">
+        <v>1</v>
+      </c>
+      <c r="H803" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="n">
+        <v>14</v>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Oregon</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>Oregon State</t>
+        </is>
+      </c>
+      <c r="D804" t="inlineStr"/>
+      <c r="E804" t="n">
+        <v>0</v>
+      </c>
+      <c r="F804" t="n">
+        <v>24</v>
+      </c>
+      <c r="G804" t="n">
+        <v>1</v>
+      </c>
+      <c r="H804" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="n">
+        <v>14</v>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Penn State</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>Michigan State</t>
+        </is>
+      </c>
+      <c r="D805" t="inlineStr"/>
+      <c r="E805" t="n">
+        <v>1</v>
+      </c>
+      <c r="F805" t="n">
+        <v>42</v>
+      </c>
+      <c r="G805" t="n">
+        <v>1</v>
+      </c>
+      <c r="H805" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="n">
+        <v>14</v>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Texas</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>Texas Tech</t>
+        </is>
+      </c>
+      <c r="D806" t="inlineStr"/>
+      <c r="E806" t="n">
+        <v>0</v>
+      </c>
+      <c r="F806" t="n">
+        <v>50</v>
+      </c>
+      <c r="G806" t="n">
+        <v>1</v>
+      </c>
+      <c r="H806" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="n">
+        <v>14</v>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Central Michigan</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>Toledo</t>
+        </is>
+      </c>
+      <c r="D807" t="inlineStr"/>
+      <c r="E807" t="n">
+        <v>0</v>
+      </c>
+      <c r="F807" t="n">
+        <v>15</v>
+      </c>
+      <c r="G807" t="n">
+        <v>0</v>
+      </c>
+      <c r="H807" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="n">
+        <v>14</v>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Tulane</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>Texas-San Antonio</t>
+        </is>
+      </c>
+      <c r="D808" t="inlineStr"/>
+      <c r="E808" t="n">
+        <v>0</v>
+      </c>
+      <c r="F808" t="n">
+        <v>13</v>
+      </c>
+      <c r="G808" t="n">
+        <v>1</v>
+      </c>
+      <c r="H808" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="n">
+        <v>14</v>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>New Mexico</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>Utah State</t>
+        </is>
+      </c>
+      <c r="D809" t="inlineStr"/>
+      <c r="E809" t="n">
+        <v>0</v>
+      </c>
+      <c r="F809" t="n">
+        <v>3</v>
+      </c>
+      <c r="G809" t="n">
+        <v>0</v>
+      </c>
+      <c r="H809" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="n">
+        <v>14</v>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Auburn</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>Alabama</t>
+        </is>
+      </c>
+      <c r="D810" t="inlineStr"/>
+      <c r="E810" t="n">
+        <v>0</v>
+      </c>
+      <c r="F810" t="n">
+        <v>3</v>
+      </c>
+      <c r="G810" t="n">
+        <v>0</v>
+      </c>
+      <c r="H810" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="n">
+        <v>14</v>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Appalachian State</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>Georgia Southern</t>
+        </is>
+      </c>
+      <c r="D811" t="inlineStr"/>
+      <c r="E811" t="n">
+        <v>0</v>
+      </c>
+      <c r="F811" t="n">
+        <v>28</v>
+      </c>
+      <c r="G811" t="n">
+        <v>1</v>
+      </c>
+      <c r="H811" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="n">
+        <v>14</v>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Arizona State</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>Arizona</t>
+        </is>
+      </c>
+      <c r="D812" t="inlineStr"/>
+      <c r="E812" t="n">
+        <v>0</v>
+      </c>
+      <c r="F812" t="n">
+        <v>36</v>
+      </c>
+      <c r="G812" t="n">
+        <v>0</v>
+      </c>
+      <c r="H812" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="n">
+        <v>14</v>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>UCLA</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>California</t>
+        </is>
+      </c>
+      <c r="D813" t="inlineStr"/>
+      <c r="E813" t="n">
+        <v>0</v>
+      </c>
+      <c r="F813" t="n">
+        <v>26</v>
+      </c>
+      <c r="G813" t="n">
+        <v>0</v>
+      </c>
+      <c r="H813" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="n">
+        <v>14</v>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Central Florida</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>Houston</t>
+        </is>
+      </c>
+      <c r="D814" t="inlineStr"/>
+      <c r="E814" t="n">
+        <v>0</v>
+      </c>
+      <c r="F814" t="n">
+        <v>14</v>
+      </c>
+      <c r="G814" t="n">
+        <v>1</v>
+      </c>
+      <c r="H814" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="n">
+        <v>14</v>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>South Carolina</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>Clemson</t>
+        </is>
+      </c>
+      <c r="D815" t="inlineStr"/>
+      <c r="E815" t="n">
+        <v>0</v>
+      </c>
+      <c r="F815" t="n">
+        <v>9</v>
+      </c>
+      <c r="G815" t="n">
+        <v>0</v>
+      </c>
+      <c r="H815" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="n">
+        <v>14</v>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Massachusetts</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>Connecticut</t>
+        </is>
+      </c>
+      <c r="D816" t="inlineStr"/>
+      <c r="E816" t="n">
+        <v>0</v>
+      </c>
+      <c r="F816" t="n">
+        <v>13</v>
+      </c>
+      <c r="G816" t="n">
+        <v>0</v>
+      </c>
+      <c r="H816" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="n">
+        <v>14</v>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Duke</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>Pittsburgh</t>
+        </is>
+      </c>
+      <c r="D817" t="inlineStr"/>
+      <c r="E817" t="n">
+        <v>0</v>
+      </c>
+      <c r="F817" t="n">
+        <v>11</v>
+      </c>
+      <c r="G817" t="n">
+        <v>1</v>
+      </c>
+      <c r="H817" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="n">
+        <v>14</v>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Florida</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>Florida State</t>
+        </is>
+      </c>
+      <c r="D818" t="inlineStr"/>
+      <c r="E818" t="n">
+        <v>0</v>
+      </c>
+      <c r="F818" t="n">
+        <v>9</v>
+      </c>
+      <c r="G818" t="n">
+        <v>0</v>
+      </c>
+      <c r="H818" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="n">
+        <v>14</v>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Georgia Tech</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>Georgia</t>
+        </is>
+      </c>
+      <c r="D819" t="inlineStr"/>
+      <c r="E819" t="n">
+        <v>0</v>
+      </c>
+      <c r="F819" t="n">
+        <v>8</v>
+      </c>
+      <c r="G819" t="n">
+        <v>0</v>
+      </c>
+      <c r="H819" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="n">
+        <v>14</v>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Hawaii</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>Colorado State</t>
+        </is>
+      </c>
+      <c r="D820" t="inlineStr"/>
+      <c r="E820" t="n">
+        <v>0</v>
+      </c>
+      <c r="F820" t="n">
+        <v>3</v>
+      </c>
+      <c r="G820" t="n">
+        <v>1</v>
+      </c>
+      <c r="H820" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="n">
+        <v>14</v>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Kansas State</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>Iowa State</t>
+        </is>
+      </c>
+      <c r="D821" t="inlineStr"/>
+      <c r="E821" t="n">
+        <v>0</v>
+      </c>
+      <c r="F821" t="n">
+        <v>7</v>
+      </c>
+      <c r="G821" t="n">
+        <v>0</v>
+      </c>
+      <c r="H821" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="n">
+        <v>14</v>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Coastal Carolina</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>James Madison</t>
+        </is>
+      </c>
+      <c r="D822" t="inlineStr"/>
+      <c r="E822" t="n">
+        <v>0</v>
+      </c>
+      <c r="F822" t="n">
+        <v>42</v>
+      </c>
+      <c r="G822" t="n">
+        <v>0</v>
+      </c>
+      <c r="H822" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="n">
+        <v>14</v>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Cincinnati</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>Kansas</t>
+        </is>
+      </c>
+      <c r="D823" t="inlineStr"/>
+      <c r="E823" t="n">
+        <v>0</v>
+      </c>
+      <c r="F823" t="n">
+        <v>33</v>
+      </c>
+      <c r="G823" t="n">
+        <v>0</v>
+      </c>
+      <c r="H823" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="n">
+        <v>14</v>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Louisville</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>Kentucky</t>
+        </is>
+      </c>
+      <c r="D824" t="inlineStr"/>
+      <c r="E824" t="n">
+        <v>0</v>
+      </c>
+      <c r="F824" t="n">
+        <v>7</v>
+      </c>
+      <c r="G824" t="n">
+        <v>0</v>
+      </c>
+      <c r="H824" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="n">
+        <v>14</v>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Texas-El Paso</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>Liberty</t>
+        </is>
+      </c>
+      <c r="D825" t="inlineStr"/>
+      <c r="E825" t="n">
+        <v>0</v>
+      </c>
+      <c r="F825" t="n">
+        <v>14</v>
+      </c>
+      <c r="G825" t="n">
+        <v>0</v>
+      </c>
+      <c r="H825" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="n">
+        <v>14</v>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Louisiana</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>Louisiana-Monroe</t>
+        </is>
+      </c>
+      <c r="D826" t="inlineStr"/>
+      <c r="E826" t="n">
+        <v>0</v>
+      </c>
+      <c r="F826" t="n">
+        <v>31</v>
+      </c>
+      <c r="G826" t="n">
+        <v>1</v>
+      </c>
+      <c r="H826" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="n">
+        <v>14</v>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Louisiana State</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>Texas A&amp;M</t>
+        </is>
+      </c>
+      <c r="D827" t="inlineStr"/>
+      <c r="E827" t="n">
+        <v>0</v>
+      </c>
+      <c r="F827" t="n">
+        <v>12</v>
+      </c>
+      <c r="G827" t="n">
+        <v>1</v>
+      </c>
+      <c r="H827" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="n">
+        <v>14</v>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Marshall</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>Arkansas State</t>
+        </is>
+      </c>
+      <c r="D828" t="inlineStr"/>
+      <c r="E828" t="n">
+        <v>0</v>
+      </c>
+      <c r="F828" t="n">
+        <v>14</v>
+      </c>
+      <c r="G828" t="n">
+        <v>1</v>
+      </c>
+      <c r="H828" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="n">
+        <v>14</v>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Rutgers</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>Maryland</t>
+        </is>
+      </c>
+      <c r="D829" t="inlineStr"/>
+      <c r="E829" t="n">
+        <v>0</v>
+      </c>
+      <c r="F829" t="n">
+        <v>18</v>
+      </c>
+      <c r="G829" t="n">
+        <v>0</v>
+      </c>
+      <c r="H829" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="n">
+        <v>14</v>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Ball State</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>Miami (OH)</t>
+        </is>
+      </c>
+      <c r="D830" t="inlineStr"/>
+      <c r="E830" t="n">
+        <v>0</v>
+      </c>
+      <c r="F830" t="n">
+        <v>2</v>
+      </c>
+      <c r="G830" t="n">
+        <v>0</v>
+      </c>
+      <c r="H830" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="n">
+        <v>14</v>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Michigan</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>Ohio State</t>
+        </is>
+      </c>
+      <c r="D831" t="inlineStr"/>
+      <c r="E831" t="n">
+        <v>0</v>
+      </c>
+      <c r="F831" t="n">
+        <v>6</v>
+      </c>
+      <c r="G831" t="n">
+        <v>1</v>
+      </c>
+      <c r="H831" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="n">
+        <v>14</v>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>New Mexico State</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>Jacksonville State</t>
+        </is>
+      </c>
+      <c r="D832" t="inlineStr"/>
+      <c r="E832" t="n">
+        <v>0</v>
+      </c>
+      <c r="F832" t="n">
+        <v>3</v>
+      </c>
+      <c r="G832" t="n">
+        <v>1</v>
+      </c>
+      <c r="H832" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="n">
+        <v>14</v>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>North Carolina State</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>North Carolina</t>
+        </is>
+      </c>
+      <c r="D833" t="inlineStr"/>
+      <c r="E833" t="n">
+        <v>0</v>
+      </c>
+      <c r="F833" t="n">
+        <v>19</v>
+      </c>
+      <c r="G833" t="n">
+        <v>1</v>
+      </c>
+      <c r="H833" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="n">
+        <v>14</v>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>North Texas</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>Alabama-Birmingham</t>
+        </is>
+      </c>
+      <c r="D834" t="inlineStr"/>
+      <c r="E834" t="n">
+        <v>0</v>
+      </c>
+      <c r="F834" t="n">
+        <v>3</v>
+      </c>
+      <c r="G834" t="n">
+        <v>1</v>
+      </c>
+      <c r="H834" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="n">
+        <v>14</v>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Kent State</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>Northern Illinois</t>
+        </is>
+      </c>
+      <c r="D835" t="inlineStr"/>
+      <c r="E835" t="n">
+        <v>0</v>
+      </c>
+      <c r="F835" t="n">
+        <v>10</v>
+      </c>
+      <c r="G835" t="n">
+        <v>0</v>
+      </c>
+      <c r="H835" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="n">
+        <v>14</v>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Illinois</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>Northwestern</t>
+        </is>
+      </c>
+      <c r="D836" t="inlineStr"/>
+      <c r="E836" t="n">
+        <v>0</v>
+      </c>
+      <c r="F836" t="n">
+        <v>2</v>
+      </c>
+      <c r="G836" t="n">
+        <v>0</v>
+      </c>
+      <c r="H836" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="n">
+        <v>14</v>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Stanford</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>Notre Dame</t>
+        </is>
+      </c>
+      <c r="D837" t="inlineStr"/>
+      <c r="E837" t="n">
+        <v>0</v>
+      </c>
+      <c r="F837" t="n">
+        <v>33</v>
+      </c>
+      <c r="G837" t="n">
+        <v>0</v>
+      </c>
+      <c r="H837" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="n">
+        <v>14</v>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Oklahoma State</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>Brigham Young</t>
+        </is>
+      </c>
+      <c r="D838" t="inlineStr"/>
+      <c r="E838" t="n">
+        <v>0</v>
+      </c>
+      <c r="F838" t="n">
+        <v>6</v>
+      </c>
+      <c r="G838" t="n">
+        <v>1</v>
+      </c>
+      <c r="H838" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="n">
+        <v>14</v>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Old Dominion</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>Georgia State</t>
+        </is>
+      </c>
+      <c r="D839" t="inlineStr"/>
+      <c r="E839" t="n">
+        <v>0</v>
+      </c>
+      <c r="F839" t="n">
+        <v>1</v>
+      </c>
+      <c r="G839" t="n">
+        <v>1</v>
+      </c>
+      <c r="H839" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="n">
+        <v>14</v>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Purdue</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>Indiana</t>
+        </is>
+      </c>
+      <c r="D840" t="inlineStr"/>
+      <c r="E840" t="n">
+        <v>0</v>
+      </c>
+      <c r="F840" t="n">
+        <v>4</v>
+      </c>
+      <c r="G840" t="n">
+        <v>1</v>
+      </c>
+      <c r="H840" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="n">
+        <v>14</v>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Rice</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>Florida Atlantic</t>
+        </is>
+      </c>
+      <c r="D841" t="inlineStr"/>
+      <c r="E841" t="n">
+        <v>0</v>
+      </c>
+      <c r="F841" t="n">
+        <v>3</v>
+      </c>
+      <c r="G841" t="n">
+        <v>1</v>
+      </c>
+      <c r="H841" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="n">
+        <v>14</v>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Sam Houston</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>Middle Tennessee State</t>
+        </is>
+      </c>
+      <c r="D842" t="inlineStr"/>
+      <c r="E842" t="n">
+        <v>0</v>
+      </c>
+      <c r="F842" t="n">
+        <v>3</v>
+      </c>
+      <c r="G842" t="n">
+        <v>1</v>
+      </c>
+      <c r="H842" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="n">
+        <v>14</v>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>San Diego State</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>Fresno State</t>
+        </is>
+      </c>
+      <c r="D843" t="inlineStr"/>
+      <c r="E843" t="n">
+        <v>0</v>
+      </c>
+      <c r="F843" t="n">
+        <v>15</v>
+      </c>
+      <c r="G843" t="n">
+        <v>1</v>
+      </c>
+      <c r="H843" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="n">
+        <v>14</v>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Nevada-Las Vegas</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>San Jose State</t>
+        </is>
+      </c>
+      <c r="D844" t="inlineStr"/>
+      <c r="E844" t="n">
+        <v>0</v>
+      </c>
+      <c r="F844" t="n">
+        <v>6</v>
+      </c>
+      <c r="G844" t="n">
+        <v>0</v>
+      </c>
+      <c r="H844" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="n">
+        <v>14</v>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>South Florida</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>Charlotte</t>
+        </is>
+      </c>
+      <c r="D845" t="inlineStr"/>
+      <c r="E845" t="n">
+        <v>0</v>
+      </c>
+      <c r="F845" t="n">
+        <v>34</v>
+      </c>
+      <c r="G845" t="n">
+        <v>1</v>
+      </c>
+      <c r="H845" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="n">
+        <v>14</v>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Southern Methodist</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>Navy</t>
+        </is>
+      </c>
+      <c r="D846" t="inlineStr"/>
+      <c r="E846" t="n">
+        <v>0</v>
+      </c>
+      <c r="F846" t="n">
+        <v>45</v>
+      </c>
+      <c r="G846" t="n">
+        <v>1</v>
+      </c>
+      <c r="H846" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="n">
+        <v>14</v>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Syracuse</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>Wake Forest</t>
+        </is>
+      </c>
+      <c r="D847" t="inlineStr"/>
+      <c r="E847" t="n">
+        <v>0</v>
+      </c>
+      <c r="F847" t="n">
+        <v>4</v>
+      </c>
+      <c r="G847" t="n">
+        <v>1</v>
+      </c>
+      <c r="H847" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="n">
+        <v>14</v>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Tennessee</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>Vanderbilt</t>
+        </is>
+      </c>
+      <c r="D848" t="inlineStr"/>
+      <c r="E848" t="n">
+        <v>0</v>
+      </c>
+      <c r="F848" t="n">
+        <v>24</v>
+      </c>
+      <c r="G848" t="n">
+        <v>1</v>
+      </c>
+      <c r="H848" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="n">
+        <v>14</v>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Texas State</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>South Alabama</t>
+        </is>
+      </c>
+      <c r="D849" t="inlineStr"/>
+      <c r="E849" t="n">
+        <v>0</v>
+      </c>
+      <c r="F849" t="n">
+        <v>8</v>
+      </c>
+      <c r="G849" t="n">
+        <v>1</v>
+      </c>
+      <c r="H849" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="n">
+        <v>14</v>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Southern Mississippi</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>Troy</t>
+        </is>
+      </c>
+      <c r="D850" t="inlineStr"/>
+      <c r="E850" t="n">
+        <v>0</v>
+      </c>
+      <c r="F850" t="n">
+        <v>18</v>
+      </c>
+      <c r="G850" t="n">
+        <v>0</v>
+      </c>
+      <c r="H850" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="n">
+        <v>14</v>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>East Carolina</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>Tulsa</t>
+        </is>
+      </c>
+      <c r="D851" t="inlineStr"/>
+      <c r="E851" t="n">
+        <v>0</v>
+      </c>
+      <c r="F851" t="n">
+        <v>2</v>
+      </c>
+      <c r="G851" t="n">
+        <v>0</v>
+      </c>
+      <c r="H851" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="n">
+        <v>14</v>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Utah</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>Colorado</t>
+        </is>
+      </c>
+      <c r="D852" t="inlineStr"/>
+      <c r="E852" t="n">
+        <v>0</v>
+      </c>
+      <c r="F852" t="n">
+        <v>6</v>
+      </c>
+      <c r="G852" t="n">
+        <v>1</v>
+      </c>
+      <c r="H852" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="n">
+        <v>14</v>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Virginia</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>Virginia Tech</t>
+        </is>
+      </c>
+      <c r="D853" t="inlineStr"/>
+      <c r="E853" t="n">
+        <v>0</v>
+      </c>
+      <c r="F853" t="n">
+        <v>38</v>
+      </c>
+      <c r="G853" t="n">
+        <v>0</v>
+      </c>
+      <c r="H853" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="n">
+        <v>14</v>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Washington</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>Washington State</t>
+        </is>
+      </c>
+      <c r="D854" t="inlineStr"/>
+      <c r="E854" t="n">
+        <v>0</v>
+      </c>
+      <c r="F854" t="n">
+        <v>3</v>
+      </c>
+      <c r="G854" t="n">
+        <v>1</v>
+      </c>
+      <c r="H854" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="n">
+        <v>14</v>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Baylor</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>West Virginia</t>
+        </is>
+      </c>
+      <c r="D855" t="inlineStr"/>
+      <c r="E855" t="n">
+        <v>0</v>
+      </c>
+      <c r="F855" t="n">
+        <v>3</v>
+      </c>
+      <c r="G855" t="n">
+        <v>0</v>
+      </c>
+      <c r="H855" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="n">
+        <v>14</v>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Florida International</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>Western Kentucky</t>
+        </is>
+      </c>
+      <c r="D856" t="inlineStr"/>
+      <c r="E856" t="n">
+        <v>0</v>
+      </c>
+      <c r="F856" t="n">
+        <v>13</v>
+      </c>
+      <c r="G856" t="n">
+        <v>0</v>
+      </c>
+      <c r="H856" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="n">
+        <v>14</v>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Minnesota</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>Wisconsin</t>
+        </is>
+      </c>
+      <c r="D857" t="inlineStr"/>
+      <c r="E857" t="n">
+        <v>0</v>
+      </c>
+      <c r="F857" t="n">
+        <v>14</v>
+      </c>
+      <c r="G857" t="n">
+        <v>0</v>
+      </c>
+      <c r="H857" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="n">
+        <v>14</v>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Nevada</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>Wyoming</t>
+        </is>
+      </c>
+      <c r="D858" t="inlineStr"/>
+      <c r="E858" t="n">
+        <v>0</v>
+      </c>
+      <c r="F858" t="n">
+        <v>36</v>
+      </c>
+      <c r="G858" t="n">
+        <v>0</v>
+      </c>
+      <c r="H858" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>